<commit_message>
Doan day code sua danh muc hang hoa
</commit_message>
<xml_diff>
--- a/Document/5.Reference/190407_VNC_DanhSachSuaDoi.xlsx
+++ b/Document/5.Reference/190407_VNC_DanhSachSuaDoi.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21425"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{853EB9A8-6301-4F76-8261-500967CB5995}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB96BE70-D324-4FFB-ACDA-72D1C8B52DE8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="20" windowWidth="19180" windowHeight="10180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="36">
   <si>
     <t>TT</t>
   </si>
@@ -127,12 +127,21 @@
   <si>
     <t>DuyOT</t>
   </si>
+  <si>
+    <t>Tình trạng</t>
+  </si>
+  <si>
+    <t>Đã hoàn thành</t>
+  </si>
+  <si>
+    <t>Đang thực hiện</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,6 +156,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -215,7 +231,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -226,12 +242,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -242,6 +252,13 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -580,10 +597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -591,39 +608,43 @@
     <col min="1" max="1" width="6.26953125" customWidth="1"/>
     <col min="2" max="2" width="27" customWidth="1"/>
     <col min="3" max="3" width="48.08984375" customWidth="1"/>
-    <col min="4" max="4" width="15.90625" customWidth="1"/>
-    <col min="5" max="5" width="16.26953125" customWidth="1"/>
-    <col min="6" max="6" width="12.26953125" customWidth="1"/>
+    <col min="4" max="5" width="15.90625" customWidth="1"/>
+    <col min="6" max="6" width="16.26953125" customWidth="1"/>
+    <col min="7" max="7" width="12.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-    </row>
-    <row r="2" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="9" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+    </row>
+    <row r="2" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="10" t="s">
+      <c r="C2" s="7"/>
+      <c r="D2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="G2" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -636,12 +657,15 @@
       <c r="D3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="11" t="s">
+      <c r="E3" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -654,12 +678,15 @@
       <c r="D4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="11" t="s">
+      <c r="E4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -672,12 +699,15 @@
       <c r="D5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="11" t="s">
+      <c r="E5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -691,11 +721,12 @@
         <v>28</v>
       </c>
       <c r="E6" s="1"/>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="1"/>
+      <c r="G6" s="9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -708,12 +739,13 @@
       <c r="D7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="11" t="s">
+      <c r="E7" s="2"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -726,12 +758,13 @@
       <c r="D8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="11" t="s">
+      <c r="E8" s="2"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -744,12 +777,13 @@
       <c r="D9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="11" t="s">
+      <c r="E9" s="5"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>6</v>
       </c>
@@ -762,14 +796,15 @@
       <c r="D10" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="11" t="s">
+      <c r="E10" s="5"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="9" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>